<commit_message>
Audio play at point, working with PoolManager + player animation audio
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterSFX.xlsx
+++ b/Assets/Data/Excel/MasterSFX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E16C252-8CE5-4C29-9276-8775E173D081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10751F82-D4E3-42DC-AD56-6FC70587FE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -51,9 +51,6 @@
     <t>SFX_03_ThirdAudio</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>audioSFXType</t>
   </si>
   <si>
@@ -66,7 +63,70 @@
     <t>SFX_3</t>
   </si>
   <si>
-    <t>SFX_4</t>
+    <t>PlayerFootsteps_01</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_02</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_03</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_04</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_05</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_06</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_07</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_08</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_09</t>
+  </si>
+  <si>
+    <t>PlayerFootsteps_010</t>
+  </si>
+  <si>
+    <t>PlayerLand</t>
+  </si>
+  <si>
+    <t>Player_Footstep_01</t>
+  </si>
+  <si>
+    <t>Player_Land</t>
+  </si>
+  <si>
+    <t>Player_Footstep_02</t>
+  </si>
+  <si>
+    <t>Player_Footstep_03</t>
+  </si>
+  <si>
+    <t>Player_Footstep_04</t>
+  </si>
+  <si>
+    <t>Player_Footstep_05</t>
+  </si>
+  <si>
+    <t>Player_Footstep_06</t>
+  </si>
+  <si>
+    <t>Player_Footstep_07</t>
+  </si>
+  <si>
+    <t>Player_Footstep_08</t>
+  </si>
+  <si>
+    <t>Player_Footstep_09</t>
+  </si>
+  <si>
+    <t>Player_Footstep_10</t>
   </si>
 </sst>
 </file>
@@ -418,14 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -437,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -445,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -456,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -467,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -475,13 +536,123 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>1000</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1001</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1003</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1004</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1005</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1006</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1007</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1008</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1009</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1010</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>